<commit_message>
docs: Creating API file
</commit_message>
<xml_diff>
--- a/api/Board/Free_API.xlsx
+++ b/api/Board/Free_API.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Documents\GitHub\AISW_Web_Community\api\Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECED4AE0-5F18-4E13-A81E-CE74E8EB05C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C2349D-6F36-4255-AC19-48E0BF89049B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{4D31F6B6-070E-4774-AAEF-202F9D53FBBB}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="106">
   <si>
     <t>Title</t>
   </si>
@@ -856,6 +856,35 @@
   </si>
   <si>
     <t>Board DB Index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Data </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>부</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 리스트</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>List&lt;Object&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -948,6 +977,7 @@
       "status": "GENERAL",
       "views" : 1,
       "likes" : 1,
+      "is_anonymous" : "true",
       "created_at" : "2021-01-01T01:01:11.111",
       "created_by" : "Hong gil dong",
       "updated_at" : null,
@@ -967,35 +997,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Data </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>부</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 리스트</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>List&lt;Object&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>{
    "transaction_time" : "2021-01-08T17:12:33.333",
    "result_code" : "OK",
@@ -1084,6 +1085,7 @@
       "status": "GENERAL",
       "views" : 1,
       "likes" : 1,
+      "is_anonymous" : "true",
       "created_at" : "2021-01-01T01:01:11.111",
       "created_by" : "Hong gil dong",
       "updated_at" : null,
@@ -1184,6 +1186,7 @@
       "status": "GENERAL",
       "views" : 1,
       "likes" : 1,
+      "is_anonymous" : "true",
       "level" : 0,
       "user_id" : 1
    }
@@ -1281,6 +1284,7 @@
       "status": "GENERAL",
       "views" : 1,
       "likes" : 1,
+      "is_anonymous" : "true",
       "created_at" : "2021-01-01T01:01:11.111",
       "created_by" : "Hong gil dong",
       "updated_at" : null,
@@ -1288,6 +1292,68 @@
       "level" : 0
    }
 }</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>익명여부</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is_anonymous</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>익명</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> true, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>비익명</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> false</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1458,7 +1524,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1527,17 +1593,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1547,7 +1602,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1606,22 +1661,38 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1632,13 +1703,16 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1668,21 +1742,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1691,6 +1750,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1708,12 +1773,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -2031,8 +2090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B60143-E3B9-4AB4-9B51-6040CE152FCC}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2047,95 +2106,95 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -2184,64 +2243,64 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="32"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
@@ -2323,14 +2382,14 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="F20" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G20" s="22" t="s">
         <v>21</v>
@@ -2440,7 +2499,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A26" s="61" t="s">
+      <c r="A26" s="27" t="s">
         <v>92</v>
       </c>
       <c r="B26" s="8"/>
@@ -2460,54 +2519,57 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A27" s="60" t="s">
+      <c r="A27" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="60" t="s">
+      <c r="B27" s="24"/>
+      <c r="C27" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="F27" s="60" t="s">
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="G27" s="60" t="s">
+      <c r="G27" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="H27" s="60" t="s">
+      <c r="H27" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="8"/>
+        <v>102</v>
+      </c>
+      <c r="B28" s="24"/>
       <c r="C28" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="8"/>
+        <v>103</v>
+      </c>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
       <c r="F28" s="8" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>21</v>
@@ -2518,34 +2580,36 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H30" s="8"/>
+        <v>21</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>32</v>
@@ -2553,78 +2617,86 @@
       <c r="H31" s="8"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="10"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H32" s="8"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A33" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22" t="s">
+      <c r="B33" s="25"/>
+      <c r="C33" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22" t="s">
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G32" s="22" t="s">
+      <c r="G33" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H32" s="22" t="s">
+      <c r="H33" s="25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A33" s="22" t="s">
+    <row r="34" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22" t="s">
+      <c r="B34" s="25"/>
+      <c r="C34" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22" t="s">
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G33" s="22" t="s">
+      <c r="G34" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H33" s="22" t="s">
+      <c r="H34" s="25" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="34" t="s">
+    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="35"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="36"/>
-    </row>
-    <row r="35" spans="1:8" ht="349.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="B35" s="47"/>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="48"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="33"/>
+    </row>
+    <row r="36" spans="1:8" ht="409.6" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="30"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="11"/>
@@ -3188,20 +3260,20 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
     <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A34:H34"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="A11:H11"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="B15:H15"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -3216,8 +3288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA89CF2D-BC52-4BF4-868E-5B8B099A5517}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -3232,95 +3304,95 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="39"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="46"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -3379,64 +3451,64 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="32"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="21" t="s">
@@ -3635,7 +3707,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A26" s="61" t="s">
+      <c r="A26" s="27" t="s">
         <v>92</v>
       </c>
       <c r="B26" s="8"/>
@@ -3655,54 +3727,57 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A27" s="60" t="s">
+      <c r="A27" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="60" t="s">
+      <c r="B27" s="24"/>
+      <c r="C27" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="F27" s="60" t="s">
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="G27" s="60" t="s">
+      <c r="G27" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="H27" s="60" t="s">
+      <c r="H27" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="8"/>
+        <v>102</v>
+      </c>
+      <c r="B28" s="24"/>
       <c r="C28" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="8"/>
+        <v>103</v>
+      </c>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
       <c r="F28" s="8" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>21</v>
@@ -3713,34 +3788,36 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H30" s="8"/>
+        <v>21</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>32</v>
@@ -3748,78 +3825,86 @@
       <c r="H31" s="8"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="10"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H32" s="8"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A33" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22" t="s">
+      <c r="B33" s="25"/>
+      <c r="C33" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22" t="s">
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G32" s="22" t="s">
+      <c r="G33" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H32" s="22" t="s">
+      <c r="H33" s="25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A33" s="22" t="s">
+    <row r="34" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22" t="s">
+      <c r="B34" s="25"/>
+      <c r="C34" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22" t="s">
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G33" s="22" t="s">
+      <c r="G34" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H33" s="22" t="s">
+      <c r="H34" s="25" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="34" t="s">
+    <row r="35" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="35"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="36"/>
-    </row>
-    <row r="35" spans="1:8" ht="272.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="46" t="s">
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="33"/>
+    </row>
+    <row r="36" spans="1:8" ht="280" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="B35" s="47"/>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="48"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="30"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="11"/>
@@ -4383,20 +4468,20 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
     <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A34:H34"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="A11:H11"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="B15:H15"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -4411,8 +4496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B31E2576-20FD-4E47-B846-39903FF9702A}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD41"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -4427,95 +4512,95 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="39"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="46"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -4714,54 +4799,57 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="B18" s="24"/>
+      <c r="C18" s="8" t="s">
         <v>89</v>
       </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
       <c r="F18" s="9" t="s">
         <v>36</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="60" t="s">
+      <c r="H18" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="8"/>
+        <v>102</v>
+      </c>
+      <c r="B19" s="24"/>
       <c r="C19" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="8"/>
+        <v>103</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
       <c r="F19" s="8" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>21</v>
@@ -4772,34 +4860,36 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H21" s="8"/>
+        <v>21</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>32</v>
@@ -4807,250 +4897,248 @@
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="10"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" s="8"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22" t="s">
+      <c r="B24" s="25"/>
+      <c r="C24" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22" t="s">
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G23" s="22" t="s">
+      <c r="G24" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H23" s="22" t="s">
+      <c r="H24" s="25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A24" s="22" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22" t="s">
+      <c r="B25" s="25"/>
+      <c r="C25" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22" t="s">
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="G25" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H24" s="22" t="s">
+      <c r="H25" s="25" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A25" s="40" t="s">
+    <row r="26" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="42"/>
-    </row>
-    <row r="26" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="43" t="s">
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="49"/>
+    </row>
+    <row r="27" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="44"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="45"/>
-    </row>
-    <row r="27" spans="1:8" ht="223.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="46" t="s">
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="52"/>
+    </row>
+    <row r="28" spans="1:8" ht="303.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="B27" s="47"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="48"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A28" s="34" t="s">
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="30"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A29" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="36"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A29" s="21" t="s">
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="33"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A30" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="51" t="s">
+      <c r="B30" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="53"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A30" s="21" t="s">
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="55"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A31" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B31" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C31" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D31" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E31" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F31" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G30" s="21" t="s">
+      <c r="G31" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H30" s="21" t="s">
+      <c r="H31" s="26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A31" s="22" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A32" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22" t="s">
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="22" t="s">
+      <c r="G32" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H31" s="22" t="s">
+      <c r="H32" s="25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A32" s="22" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A33" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22" t="s">
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G32" s="22" t="s">
+      <c r="G33" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H32" s="22" t="s">
+      <c r="H33" s="25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A33" s="22" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A34" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22" t="s">
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G33" s="22" t="s">
+      <c r="G34" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="H33" s="22"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A34" s="22" t="s">
+      <c r="H34" s="25"/>
+    </row>
+    <row r="35" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22" t="s">
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="G34" s="22" t="s">
+      <c r="G35" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H34" s="22" t="s">
+      <c r="H35" s="25" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="22" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A36" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22" t="s">
+      <c r="B36" s="25"/>
+      <c r="C36" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22" t="s">
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G35" s="22" t="s">
+      <c r="G36" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H35" s="22" t="s">
+      <c r="H36" s="25" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A36" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H36" s="8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="8"/>
@@ -5061,16 +5149,16 @@
         <v>21</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A38" s="9" t="s">
-        <v>46</v>
+      <c r="A38" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D38" s="10"/>
       <c r="E38" s="8"/>
@@ -5078,116 +5166,119 @@
         <v>27</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>48</v>
+        <v>21</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A39" s="8" t="s">
-        <v>49</v>
+      <c r="A39" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H39" s="8" t="s">
-        <v>65</v>
+        <v>32</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A40" s="9" t="s">
-        <v>51</v>
+      <c r="A40" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="B40" s="8"/>
-      <c r="C40" s="9" t="s">
-        <v>52</v>
+      <c r="C40" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="8"/>
-      <c r="F40" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G40" s="9" t="s">
+      <c r="F40" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G40" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H40" s="9" t="s">
+      <c r="H40" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A41" s="60" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" s="60" t="s">
-        <v>89</v>
-      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" s="10"/>
+      <c r="E41" s="8"/>
       <c r="F41" s="9" t="s">
         <v>36</v>
       </c>
       <c r="G41" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H41" s="60" t="s">
-        <v>88</v>
+      <c r="H41" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B42" s="8"/>
+        <v>88</v>
+      </c>
+      <c r="B42" s="24"/>
       <c r="C42" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G42" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G42" s="9" t="s">
         <v>21</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B43" s="8"/>
+        <v>102</v>
+      </c>
+      <c r="B43" s="24"/>
       <c r="C43" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D43" s="10"/>
-      <c r="E43" s="8"/>
+        <v>103</v>
+      </c>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
       <c r="F43" s="8" t="s">
-        <v>27</v>
+        <v>104</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="8"/>
@@ -5195,17 +5286,19 @@
         <v>55</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H44" s="8"/>
+        <v>21</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D45" s="10"/>
       <c r="E45" s="8"/>
@@ -5213,73 +5306,111 @@
         <v>27</v>
       </c>
       <c r="G45" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A46" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" s="10"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G46" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H45" s="8"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A46" s="22" t="s">
+      <c r="H46" s="8"/>
+    </row>
+    <row r="47" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D47" s="10"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H47" s="8"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A48" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B46" s="22"/>
-      <c r="C46" s="22" t="s">
+      <c r="B48" s="25"/>
+      <c r="C48" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22" t="s">
+      <c r="D48" s="25"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G46" s="22" t="s">
+      <c r="G48" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H46" s="22" t="s">
+      <c r="H48" s="25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="22" t="s">
+    <row r="49" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22" t="s">
+      <c r="B49" s="25"/>
+      <c r="C49" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22" t="s">
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G47" s="22" t="s">
+      <c r="G49" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H47" s="22" t="s">
+      <c r="H49" s="25" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A48" s="34" t="s">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A50" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B48" s="35"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="35"/>
-      <c r="H48" s="36"/>
-    </row>
-    <row r="49" spans="1:8" ht="271" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="46" t="s">
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="33"/>
+    </row>
+    <row r="51" spans="1:8" ht="391" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="47"/>
-      <c r="C49" s="47"/>
-      <c r="D49" s="47"/>
-      <c r="E49" s="47"/>
-      <c r="F49" s="47"/>
-      <c r="G49" s="47"/>
-      <c r="H49" s="48"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="30"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" s="13"/>
@@ -5603,13 +5734,8 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A48:H48"/>
-    <mergeCell ref="A49:H49"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="A50:H50"/>
+    <mergeCell ref="A51:H51"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
@@ -5617,11 +5743,16 @@
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{3A039392-055F-41DA-91B1-F0EA51FC2A4E}"/>
-    <hyperlink ref="A26" r:id="rId2" xr:uid="{364A12D2-4995-4A23-A404-6A0D1A2185AC}"/>
+    <hyperlink ref="A27" r:id="rId2" xr:uid="{364A12D2-4995-4A23-A404-6A0D1A2185AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5631,8 +5762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAE31BB7-A599-4ABB-A50D-5795B880F93B}">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:XFD51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -5647,95 +5778,95 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="39"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="46"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -5954,54 +6085,57 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="60" t="s">
+      <c r="B19" s="24"/>
+      <c r="C19" s="8" t="s">
         <v>89</v>
       </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
       <c r="F19" s="9" t="s">
         <v>36</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="60" t="s">
+      <c r="H19" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="8"/>
+        <v>102</v>
+      </c>
+      <c r="B20" s="24"/>
       <c r="C20" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="8"/>
+        <v>103</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
       <c r="F20" s="8" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>21</v>
@@ -6012,34 +6146,36 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H22" s="8"/>
+        <v>21</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>32</v>
@@ -6047,235 +6183,233 @@
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="8"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A25" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22" t="s">
+      <c r="B25" s="25"/>
+      <c r="C25" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22" t="s">
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="G25" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H24" s="22" t="s">
+      <c r="H25" s="25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A25" s="40" t="s">
+    <row r="26" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="42"/>
-    </row>
-    <row r="26" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="43" t="s">
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="49"/>
+    </row>
+    <row r="27" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="44"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="45"/>
-    </row>
-    <row r="27" spans="1:13" ht="265.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="46" t="s">
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="52"/>
+    </row>
+    <row r="28" spans="1:13" ht="264" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="B27" s="47"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="48"/>
-    </row>
-    <row r="28" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="34" t="s">
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="30"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A29" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="36"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A29" s="21" t="s">
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="33"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A30" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="51" t="s">
+      <c r="B30" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="53"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A30" s="21" t="s">
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="55"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A31" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B31" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C31" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D31" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E31" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F31" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G30" s="21" t="s">
+      <c r="G31" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H30" s="21" t="s">
+      <c r="H31" s="26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A31" s="22" t="s">
+    <row r="32" spans="1:13" ht="15.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22" t="s">
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="22" t="s">
+      <c r="G32" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H31" s="22" t="s">
+      <c r="H32" s="25" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" ht="15.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="22" t="s">
+      <c r="I32" s="56"/>
+      <c r="J32" s="57"/>
+      <c r="K32" s="57"/>
+      <c r="L32" s="57"/>
+      <c r="M32" s="57"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A33" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22" t="s">
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G32" s="22" t="s">
+      <c r="G33" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H32" s="22" t="s">
+      <c r="H33" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="I32" s="49"/>
-      <c r="J32" s="50"/>
-      <c r="K32" s="50"/>
-      <c r="L32" s="50"/>
-      <c r="M32" s="50"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A33" s="22" t="s">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A34" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22" t="s">
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G33" s="22" t="s">
+      <c r="G34" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="H33" s="22"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A34" s="22" t="s">
+      <c r="H34" s="25"/>
+    </row>
+    <row r="35" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22" t="s">
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="G34" s="22" t="s">
+      <c r="G35" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H34" s="22" t="s">
+      <c r="H35" s="25" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="22" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A36" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22" t="s">
+      <c r="B36" s="25"/>
+      <c r="C36" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22" t="s">
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G35" s="22" t="s">
+      <c r="G36" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H35" s="22" t="s">
+      <c r="H36" s="25" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A36" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H36" s="8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="8"/>
@@ -6286,16 +6420,16 @@
         <v>21</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A38" s="9" t="s">
-        <v>46</v>
+      <c r="A38" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D38" s="10"/>
       <c r="E38" s="8"/>
@@ -6303,116 +6437,119 @@
         <v>27</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>48</v>
+        <v>21</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A39" s="8" t="s">
-        <v>49</v>
+      <c r="A39" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H39" s="8" t="s">
-        <v>65</v>
+        <v>32</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A40" s="9" t="s">
-        <v>51</v>
+      <c r="A40" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="B40" s="8"/>
-      <c r="C40" s="9" t="s">
-        <v>52</v>
+      <c r="C40" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="8"/>
-      <c r="F40" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G40" s="9" t="s">
+      <c r="F40" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G40" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H40" s="9" t="s">
+      <c r="H40" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A41" s="9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A41" s="60" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" s="60" t="s">
-        <v>89</v>
-      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" s="10"/>
+      <c r="E41" s="8"/>
       <c r="F41" s="9" t="s">
         <v>36</v>
       </c>
       <c r="G41" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H41" s="60" t="s">
-        <v>88</v>
+      <c r="H41" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B42" s="8"/>
+        <v>88</v>
+      </c>
+      <c r="B42" s="24"/>
       <c r="C42" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G42" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G42" s="9" t="s">
         <v>21</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B43" s="8"/>
+        <v>102</v>
+      </c>
+      <c r="B43" s="24"/>
       <c r="C43" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D43" s="10"/>
-      <c r="E43" s="8"/>
+        <v>103</v>
+      </c>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
       <c r="F43" s="8" t="s">
-        <v>27</v>
+        <v>104</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="8"/>
@@ -6420,17 +6557,19 @@
         <v>55</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H44" s="8"/>
+        <v>21</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D45" s="10"/>
       <c r="E45" s="8"/>
@@ -6438,75 +6577,112 @@
         <v>27</v>
       </c>
       <c r="G45" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A46" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" s="10"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G46" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H45" s="8"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A46" s="22" t="s">
+      <c r="H46" s="8"/>
+    </row>
+    <row r="47" spans="1:8" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D47" s="10"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H47" s="8"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A48" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B46" s="22"/>
-      <c r="C46" s="22" t="s">
+      <c r="B48" s="25"/>
+      <c r="C48" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22" t="s">
+      <c r="D48" s="25"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G46" s="22" t="s">
+      <c r="G48" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H46" s="22" t="s">
+      <c r="H48" s="25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="22" t="s">
+    <row r="49" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22" t="s">
+      <c r="B49" s="25"/>
+      <c r="C49" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22" t="s">
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G47" s="22" t="s">
+      <c r="G49" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H47" s="22" t="s">
+      <c r="H49" s="25" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A48" s="34" t="s">
+    <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B48" s="35"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="35"/>
-      <c r="H48" s="36"/>
-    </row>
-    <row r="49" spans="1:8" ht="277" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="46" t="s">
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="33"/>
+    </row>
+    <row r="51" spans="1:8" ht="391" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="47"/>
-      <c r="C49" s="47"/>
-      <c r="D49" s="47"/>
-      <c r="E49" s="47"/>
-      <c r="F49" s="47"/>
-      <c r="G49" s="47"/>
-      <c r="H49" s="48"/>
-    </row>
-    <row r="50" spans="1:8" ht="271" customHeight="1" x14ac:dyDescent="0.45"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="30"/>
+    </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
@@ -6829,14 +7005,8 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A48:H48"/>
-    <mergeCell ref="A49:H49"/>
-    <mergeCell ref="I32:M32"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="A50:H50"/>
+    <mergeCell ref="A51:H51"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
@@ -6844,11 +7014,17 @@
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="A6:H6"/>
+    <mergeCell ref="I32:M32"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{26F60CE5-D601-4B2A-BA26-C5CDFC97ECD4}"/>
-    <hyperlink ref="A26" r:id="rId2" xr:uid="{EED67366-FBCF-48F6-BE02-C9FD51C451F4}"/>
+    <hyperlink ref="A27" r:id="rId2" xr:uid="{EED67366-FBCF-48F6-BE02-C9FD51C451F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6874,95 +7050,95 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="39"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="46"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -7011,64 +7187,64 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="42"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="49"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="45"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="52"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="56"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="58"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="62"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="36"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="33"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="53"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="55"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
@@ -7151,28 +7327,28 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
     </row>
     <row r="20" spans="1:8" ht="74" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="47"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="48"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="30"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="13"/>
@@ -7295,24 +7471,24 @@
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A33" s="54"/>
-      <c r="B33" s="54"/>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="54"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="58"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A34" s="55"/>
-      <c r="B34" s="55"/>
-      <c r="C34" s="55"/>
-      <c r="D34" s="55"/>
-      <c r="E34" s="55"/>
-      <c r="F34" s="55"/>
-      <c r="G34" s="55"/>
-      <c r="H34" s="55"/>
+      <c r="A34" s="59"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="59"/>
     </row>
     <row r="35" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="17"/>
@@ -7916,13 +8092,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="B14:H14"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="A11:H11"/>
@@ -7932,6 +8101,13 @@
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="B14:H14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
feat: Modifying board api
</commit_message>
<xml_diff>
--- a/api/Board/Free_API.xlsx
+++ b/api/Board/Free_API.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Documents\GitHub\AISW_Web_Community\api\Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C2349D-6F36-4255-AC19-48E0BF89049B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C136F692-7359-4FF0-8F22-C1E619005A66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{4D31F6B6-070E-4774-AAEF-202F9D53FBBB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{4D31F6B6-070E-4774-AAEF-202F9D53FBBB}"/>
   </bookViews>
   <sheets>
     <sheet name="자유게시판 전체 조회" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="106">
   <si>
     <t>Title</t>
   </si>
@@ -1602,7 +1602,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1671,6 +1671,9 @@
     <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1679,6 +1682,19 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1692,7 +1708,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1701,18 +1716,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2091,7 +2094,7 @@
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2106,95 +2109,95 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -2243,64 +2246,64 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="38"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
@@ -2654,79 +2657,69 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="25" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A34" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G34" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25" t="s">
+      <c r="B35" s="25"/>
+      <c r="C35" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25" t="s">
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G34" s="25" t="s">
+      <c r="G35" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H34" s="25" t="s">
+      <c r="H35" s="25" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="31" t="s">
+    <row r="36" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="33"/>
-    </row>
-    <row r="36" spans="1:8" ht="409.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="28" t="s">
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="39"/>
+    </row>
+    <row r="37" spans="1:8" ht="387.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="30"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A39" s="17"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="31"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="17"/>
@@ -3260,14 +3253,14 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="A37:H37"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
-    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A36:H36"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="A11:H11"/>
     <mergeCell ref="A12:H12"/>
@@ -3289,7 +3282,7 @@
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -3304,95 +3297,95 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -3451,64 +3444,64 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="38"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="21" t="s">
@@ -3862,79 +3855,69 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="25" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A34" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G34" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25" t="s">
+      <c r="B35" s="25"/>
+      <c r="C35" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25" t="s">
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G34" s="25" t="s">
+      <c r="G35" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H34" s="25" t="s">
+      <c r="H35" s="25" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="31" t="s">
+    <row r="36" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="33"/>
-    </row>
-    <row r="36" spans="1:8" ht="280" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="28" t="s">
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="39"/>
+    </row>
+    <row r="37" spans="1:8" ht="354.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="30"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A39" s="17"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="31"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="17"/>
@@ -4468,14 +4451,14 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="A37:H37"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
-    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A36:H36"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="A11:H11"/>
     <mergeCell ref="A12:H12"/>
@@ -4496,8 +4479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B31E2576-20FD-4E47-B846-39903FF9702A}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -4512,95 +4495,95 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -4934,87 +4917,67 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A25" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="G25" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25" s="25" t="s">
-        <v>75</v>
-      </c>
-    </row>
     <row r="26" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="47" t="s">
+      <c r="A26" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="50"/>
     </row>
     <row r="27" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="50" t="s">
+      <c r="A27" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="52"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="53"/>
     </row>
     <row r="28" spans="1:8" ht="303.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="30"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="31"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="33"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="39"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="53" t="s">
+      <c r="B30" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="56"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="26" t="s">
@@ -5368,13 +5331,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" s="25" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="B49" s="25"/>
       <c r="C49" s="25" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="D49" s="25"/>
       <c r="E49" s="25"/>
@@ -5385,32 +5348,52 @@
         <v>21</v>
       </c>
       <c r="H49" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A50" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="G50" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="H50" s="25" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A50" s="31" t="s">
+    <row r="51" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="33"/>
-    </row>
-    <row r="51" spans="1:8" ht="391" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="28" t="s">
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="38"/>
+      <c r="E51" s="38"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="38"/>
+      <c r="H51" s="39"/>
+    </row>
+    <row r="52" spans="1:8" ht="358.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="29"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="29"/>
-      <c r="H51" s="30"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="30"/>
+      <c r="G52" s="30"/>
+      <c r="H52" s="31"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" s="13"/>
@@ -5734,8 +5717,8 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A50:H50"/>
     <mergeCell ref="A51:H51"/>
+    <mergeCell ref="A52:H52"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
@@ -5762,7 +5745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAE31BB7-A599-4ABB-A50D-5795B880F93B}">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
       <selection activeCell="A51" sqref="A51:XFD51"/>
     </sheetView>
   </sheetViews>
@@ -5778,95 +5761,95 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -6221,66 +6204,66 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="47" t="s">
+      <c r="A26" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="50"/>
     </row>
     <row r="27" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="50" t="s">
+      <c r="A27" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="52"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="53"/>
     </row>
     <row r="28" spans="1:13" ht="264" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="30"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="31"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="33"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="39"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="53" t="s">
+      <c r="B30" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="56"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="26" t="s">
@@ -6325,11 +6308,11 @@
       <c r="H32" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="I32" s="56"/>
-      <c r="J32" s="57"/>
-      <c r="K32" s="57"/>
-      <c r="L32" s="57"/>
-      <c r="M32" s="57"/>
+      <c r="I32" s="57"/>
+      <c r="J32" s="58"/>
+      <c r="K32" s="58"/>
+      <c r="L32" s="58"/>
+      <c r="M32" s="58"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="25" t="s">
@@ -6639,49 +6622,69 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="25" t="s">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A49" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" s="28"/>
+      <c r="C49" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G49" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H49" s="28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25" t="s">
+      <c r="B50" s="25"/>
+      <c r="C50" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25" t="s">
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G49" s="25" t="s">
+      <c r="G50" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H49" s="25" t="s">
+      <c r="H50" s="25" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="31" t="s">
+    <row r="51" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="33"/>
-    </row>
-    <row r="51" spans="1:8" ht="391" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="28" t="s">
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="38"/>
+      <c r="E51" s="38"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="38"/>
+      <c r="H51" s="39"/>
+    </row>
+    <row r="52" spans="1:8" ht="375" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="29"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="29"/>
-      <c r="H51" s="30"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="30"/>
+      <c r="G52" s="30"/>
+      <c r="H52" s="31"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" s="13"/>
@@ -7005,8 +7008,14 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A50:H50"/>
+    <mergeCell ref="I32:M32"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="A51:H51"/>
+    <mergeCell ref="A52:H52"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
@@ -7014,12 +7023,6 @@
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="A6:H6"/>
-    <mergeCell ref="I32:M32"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -7034,7 +7037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE8F0A6-CE1B-4868-9054-B38C338BA073}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11:H11"/>
     </sheetView>
   </sheetViews>
@@ -7050,95 +7053,95 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -7187,64 +7190,64 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="49"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="52"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="53"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="60"/>
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="62"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="63"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="33"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="39"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="55"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="56"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
@@ -7327,28 +7330,28 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="63"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="63"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="64"/>
     </row>
     <row r="20" spans="1:8" ht="74" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="30"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="31"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="13"/>
@@ -7471,24 +7474,24 @@
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A33" s="58"/>
-      <c r="B33" s="58"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="58"/>
+      <c r="A33" s="59"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A34" s="59"/>
-      <c r="B34" s="59"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="59"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="59"/>
-      <c r="H34" s="59"/>
+      <c r="A34" s="60"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="60"/>
+      <c r="H34" s="60"/>
     </row>
     <row r="35" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="17"/>
@@ -8092,6 +8095,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="B14:H14"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="A11:H11"/>
@@ -8101,13 +8111,6 @@
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="B14:H14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>